<commit_message>
added models & some DAO functions
</commit_message>
<xml_diff>
--- a/Database_tables.xlsx
+++ b/Database_tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work\Desktop\projects\proj0\project-0-bescoto98\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work\Desktop\zero\project-0-bescoto98\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6C8F8A-03F9-431D-9C92-1A08FC46E7DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423EEE88-4FE1-4D25-8026-23C13528D377}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="18000" windowHeight="9360" xr2:uid="{8ACCB949-1489-475D-8FD7-31428F5330C3}"/>
+    <workbookView xWindow="-6495" yWindow="3210" windowWidth="5490" windowHeight="7005" xr2:uid="{8ACCB949-1489-475D-8FD7-31428F5330C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t>FN</t>
   </si>
@@ -105,6 +105,27 @@
   </si>
   <si>
     <t>zip</t>
+  </si>
+  <si>
+    <t>select * from users left join logins on users.idnum = logins.idnum;</t>
+  </si>
+  <si>
+    <t>approved</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>idnum of employee who approves it</t>
+  </si>
+  <si>
+    <t>appovals</t>
+  </si>
+  <si>
+    <t>transactionId</t>
+  </si>
+  <si>
+    <t>PK</t>
   </si>
 </sst>
 </file>
@@ -538,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D67166A-DCF1-4C1B-9FD0-EC0D57C1DA07}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,12 +570,13 @@
     <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
@@ -564,7 +586,7 @@
       </c>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -581,7 +603,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,7 +617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -609,7 +631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -619,17 +641,20 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
@@ -639,7 +664,7 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -656,7 +681,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -673,7 +698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>4</v>
       </c>
@@ -687,7 +712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="E13" s="1" t="s">
@@ -697,7 +722,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E14" s="1" t="s">
         <v>12</v>
       </c>
@@ -705,9 +730,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="6"/>
       <c r="E15" s="1" t="s">
         <v>23</v>
       </c>
@@ -715,9 +742,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
       <c r="E16" s="1" t="s">
         <v>14</v>
       </c>
@@ -726,8 +760,18 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
       <c r="E17" s="1" t="s">
         <v>13</v>
       </c>
@@ -736,12 +780,23 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
+      <c r="A18" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>

</xml_diff>

<commit_message>
changes to models & service layer
</commit_message>
<xml_diff>
--- a/Database_tables.xlsx
+++ b/Database_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work\Desktop\zero\project-0-bescoto98\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901E4BE7-CA86-460E-A610-567B22F339B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E46BE1-5F0A-4991-A54F-2735A9EC2A0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="405" windowWidth="13740" windowHeight="11820" xr2:uid="{8ACCB949-1489-475D-8FD7-31428F5330C3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{8ACCB949-1489-475D-8FD7-31428F5330C3}"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t>int</t>
   </si>
@@ -50,18 +50,12 @@
     <t>password</t>
   </si>
   <si>
-    <t>FK</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
     <t>varchar(25)</t>
   </si>
   <si>
-    <t>logins</t>
-  </si>
-  <si>
     <t>information</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
     <t>users</t>
   </si>
   <si>
-    <t>boolean</t>
-  </si>
-  <si>
     <t>PK</t>
   </si>
   <si>
@@ -95,9 +86,6 @@
     <t>money</t>
   </si>
   <si>
-    <t>PK,FK</t>
-  </si>
-  <si>
     <t xml:space="preserve">	ssn</t>
   </si>
   <si>
@@ -122,65 +110,71 @@
     <t>PK, FK</t>
   </si>
   <si>
-    <t>approvals</t>
-  </si>
-  <si>
-    <t>trans_id</t>
-  </si>
-  <si>
-    <t>approvedBy</t>
-  </si>
-  <si>
-    <t>is_approved</t>
-  </si>
-  <si>
-    <t>appr_date</t>
-  </si>
-  <si>
     <t>varchar(9)</t>
   </si>
   <si>
     <t>varchar(15)</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>Checkings or Savings</t>
   </si>
   <si>
     <t>hashed?</t>
   </si>
   <si>
+    <t>alias</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>u_type</t>
+  </si>
+  <si>
+    <t>0=admin,1=employee,2=customer</t>
+  </si>
+  <si>
+    <t>serial</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>pending, active, or canceled</t>
+  </si>
+  <si>
     <t>unique</t>
   </si>
   <si>
-    <t>set as string, cast to int to use in app</t>
-  </si>
-  <si>
-    <t>u_id of whoever approved their account, originally set null</t>
-  </si>
-  <si>
-    <t>date of approval, originally set null</t>
-  </si>
-  <si>
-    <t>alias</t>
-  </si>
-  <si>
-    <t>comments</t>
-  </si>
-  <si>
-    <t>u_type</t>
-  </si>
-  <si>
-    <t>0=admin,1=employee,2=customer</t>
+    <t>approved_by</t>
+  </si>
+  <si>
+    <t>when it was created, set to null originally</t>
+  </si>
+  <si>
+    <t>accountXref</t>
+  </si>
+  <si>
+    <t>tbID</t>
+  </si>
+  <si>
+    <t>*transactions logged, table not necessary</t>
+  </si>
+  <si>
+    <t>name of admin or employee who approved the account, set to null originally</t>
+  </si>
+  <si>
+    <t>use to allow for users to have multiple accounts &amp; joint accounts</t>
+  </si>
+  <si>
+    <t>created_on</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,8 +182,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,25 +230,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -406,19 +396,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -429,6 +410,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -745,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D67166A-DCF1-4C1B-9FD0-EC0D57C1DA07}">
   <dimension ref="B1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,31 +746,31 @@
     <col min="1" max="1" width="1" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="54.28515625" customWidth="1"/>
+    <col min="4" max="4" width="95.5703125" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="7" width="14.28515625" customWidth="1"/>
     <col min="9" max="9" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>44</v>
+      <c r="B1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="2:8" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
-      <c r="C2" s="25"/>
+      <c r="C2" s="16"/>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="11"/>
       <c r="F3" s="5"/>
@@ -786,14 +778,14 @@
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>0</v>
+      <c r="B4" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -801,7 +793,7 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1</v>
@@ -812,7 +804,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -823,115 +815,125 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="B8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="16"/>
+      <c r="B9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="5"/>
+      <c r="C12" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="B14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="5"/>
+      <c r="B15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>0</v>
+      <c r="B16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -939,28 +941,22 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -969,37 +965,41 @@
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="18" t="s">
+      <c r="B21" s="23" t="str">
+        <f>B4</f>
+        <v>u_id</v>
+      </c>
+      <c r="C21" s="24" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>1</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>1</v>
@@ -1017,38 +1017,36 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D25" s="5"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D26" s="5"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="D27" s="5"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="14" t="s">
+      <c r="B28" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D28" s="5"/>
@@ -1059,63 +1057,51 @@
       <c r="D29" s="5"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="5"/>
+      <c r="B30" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="26"/>
+      <c r="D30" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="24" t="s">
+      <c r="B31" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="D31" s="5"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="19" t="s">
+      <c r="B32" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="D32" s="5"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="6" t="s">
+      <c r="B33" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="5"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
everything ready except Testing
</commit_message>
<xml_diff>
--- a/Database_tables.xlsx
+++ b/Database_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work\Desktop\zero\project-0-bescoto98\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961BC289-449B-4D45-9F0E-1008228307C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7822FB-C741-431E-9322-B620BC6851E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15360" yWindow="3255" windowWidth="13170" windowHeight="9375" xr2:uid="{8ACCB949-1489-475D-8FD7-31428F5330C3}"/>
+    <workbookView xWindow="135" yWindow="2415" windowWidth="15705" windowHeight="9375" xr2:uid="{8ACCB949-1489-475D-8FD7-31428F5330C3}"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t>int</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Checkings or Savings</t>
   </si>
   <si>
-    <t>hashed?</t>
-  </si>
-  <si>
     <t>alias</t>
   </si>
   <si>
@@ -152,15 +149,9 @@
     <t>tbID</t>
   </si>
   <si>
-    <t>*transactions logged, table not necessary</t>
-  </si>
-  <si>
     <t>name of admin or employee who approved the account, set to null originally</t>
   </si>
   <si>
-    <t>use to allow for users to have multiple accounts &amp; joint accounts</t>
-  </si>
-  <si>
     <t>created_on</t>
   </si>
   <si>
@@ -174,6 +165,21 @@
   </si>
   <si>
     <t>account_id</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>hashed value using sha256</t>
+  </si>
+  <si>
+    <t>used to allow for users to have multiple accounts &amp; joint accounts</t>
+  </si>
+  <si>
+    <t>special characters removed before insertion and then added after retrieval</t>
+  </si>
+  <si>
+    <t>regular expressions used to verify format before insertion</t>
   </si>
 </sst>
 </file>
@@ -743,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D67166A-DCF1-4C1B-9FD0-EC0D57C1DA07}">
   <dimension ref="B1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,7 +758,7 @@
     <col min="1" max="1" width="1" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="95.5703125" customWidth="1"/>
+    <col min="4" max="4" width="80.85546875" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" customWidth="1"/>
     <col min="6" max="6" width="23.7109375" customWidth="1"/>
     <col min="7" max="7" width="19.5703125" customWidth="1"/>
@@ -762,13 +768,13 @@
   <sheetData>
     <row r="1" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="2:8" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -790,14 +796,14 @@
         <v>10</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="str">
-        <f>_xlfn.CONCAT(B4," = ?,")</f>
-        <v>u_id = ?,</v>
+        <f>_xlfn.CONCAT(B4," = ?, ")</f>
+        <v xml:space="preserve">u_id = ?, </v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -811,12 +817,12 @@
         <v>1</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" ref="E5:E9" si="0">_xlfn.CONCAT(B5," = ?,")</f>
-        <v>first_name = ?,</v>
+        <f t="shared" ref="E5:E9" si="0">_xlfn.CONCAT(B5," = ?, ")</f>
+        <v xml:space="preserve">first_name = ?, </v>
       </c>
       <c r="F5" s="5" t="str">
         <f>_xlfn.CONCAT(E4:E9)</f>
-        <v>u_id = ?,first_name = ?,last_name = ?,u_type = ?,username = ?,pass = ?,</v>
+        <v xml:space="preserve">u_id = ?, first_name = ?, last_name = ?, u_type = ?, username = ?, pass = ?, </v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -830,7 +836,7 @@
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>last_name = ?,</v>
+        <v xml:space="preserve">last_name = ?, </v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -838,17 +844,17 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>u_type = ?,</v>
+        <v xml:space="preserve">u_type = ?, </v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -862,11 +868,11 @@
         <v>1</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v>username = ?,</v>
+        <v xml:space="preserve">username = ?, </v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -874,17 +880,17 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>pass = ?,</v>
+        <v xml:space="preserve">pass = ?, </v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -911,7 +917,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>9</v>
@@ -925,7 +931,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" t="str">
@@ -959,13 +965,13 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
@@ -977,13 +983,13 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
@@ -995,13 +1001,13 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="1"/>
@@ -1033,14 +1039,6 @@
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="5"/>
-      <c r="E20" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">information= ?, </v>
-      </c>
-      <c r="F20" t="str">
-        <f>_xlfn.CONCAT(E20:E28)</f>
-        <v xml:space="preserve">information= ?, u_id= ?, 	ssn= ?, 	address= ?, 	city= ?, 	state= ?, 	zip= ?, 	phone= ?, 	email= ?, </v>
-      </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="23" t="str">
@@ -1057,6 +1055,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">u_id= ?, </v>
       </c>
+      <c r="F21" t="str">
+        <f>_xlfn.CONCAT(E21:E29)</f>
+        <v xml:space="preserve">u_id= ?, 	ssn= ?, 	address= ?, 	city= ?, 	state= ?, 	zip= ?, 	phone= ?, 	email= ?, </v>
+      </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
@@ -1130,7 +1132,9 @@
       <c r="C27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="5"/>
+      <c r="D27" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E27" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">	phone= ?, </v>
@@ -1143,7 +1147,9 @@
       <c r="C28" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="E28" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">	email= ?, </v>
@@ -1156,16 +1162,16 @@
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" s="26"/>
       <c r="D30" s="5" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" s="30" t="s">
         <v>0</v>
@@ -1174,7 +1180,7 @@
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="27" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C32" s="15" t="s">
         <v>0</v>
@@ -1183,7 +1189,7 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="28" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C33" s="29" t="s">
         <v>0</v>
@@ -1198,9 +1204,7 @@
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>

</xml_diff>

<commit_message>
everything works as required
</commit_message>
<xml_diff>
--- a/Database_tables.xlsx
+++ b/Database_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work\Desktop\zero\project-0-bescoto98\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7822FB-C741-431E-9322-B620BC6851E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264D7DC1-E193-4FB4-B762-F4CE99F5BD10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="135" yWindow="2415" windowWidth="15705" windowHeight="9375" xr2:uid="{8ACCB949-1489-475D-8FD7-31428F5330C3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>int</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>regular expressions used to verify format before insertion</t>
+  </si>
+  <si>
+    <t>FK</t>
   </si>
 </sst>
 </file>
@@ -749,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D67166A-DCF1-4C1B-9FD0-EC0D57C1DA07}">
   <dimension ref="B1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1188,9 @@
       <c r="C32" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D32" s="5"/>
+      <c r="D32" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="28" t="s">
@@ -1194,7 +1199,9 @@
       <c r="C33" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D33" s="5"/>
+      <c r="D33" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>

</xml_diff>